<commit_message>
select algorithm add (1st: Simple-rotate - 1st always home, 2nd: with check home-guest matches)
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -29,43 +29,43 @@
     <t>1 Тур</t>
   </si>
   <si>
+    <t>Петров</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Котов</t>
+  </si>
+  <si>
+    <t>Серов</t>
+  </si>
+  <si>
+    <t>Амелин</t>
+  </si>
+  <si>
+    <t>Белов</t>
+  </si>
+  <si>
+    <t>Сидоров</t>
+  </si>
+  <si>
+    <t>Кротов</t>
+  </si>
+  <si>
     <t>пропуск</t>
   </si>
   <si>
-    <t>-</t>
+    <t>Иванов</t>
   </si>
   <si>
     <t>Перов</t>
   </si>
   <si>
-    <t>Сидоров</t>
+    <t>Якин</t>
   </si>
   <si>
     <t>Уткин</t>
-  </si>
-  <si>
-    <t>Кротов</t>
-  </si>
-  <si>
-    <t>Якин</t>
-  </si>
-  <si>
-    <t>Амелин</t>
-  </si>
-  <si>
-    <t>Белов</t>
-  </si>
-  <si>
-    <t>Иванов</t>
-  </si>
-  <si>
-    <t>Серов</t>
-  </si>
-  <si>
-    <t>Петров</t>
-  </si>
-  <si>
-    <t>Котов</t>
   </si>
   <si>
     <t>2 Тур</t>
@@ -200,7 +200,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.0</v>
+        <v>840.0</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
@@ -209,7 +209,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>750.0</v>
+        <v>900.0</v>
       </c>
     </row>
     <row r="4">
@@ -220,7 +220,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>720.0</v>
+        <v>730.0</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
@@ -229,7 +229,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>750.0</v>
+        <v>680.0</v>
       </c>
     </row>
     <row r="5">
@@ -240,7 +240,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>800.0</v>
+        <v>810.0</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
@@ -249,7 +249,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>750.0</v>
+        <v>720.0</v>
       </c>
     </row>
     <row r="6">
@@ -260,7 +260,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>680.0</v>
+        <v>800.0</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>6</v>
@@ -269,7 +269,7 @@
         <v>13</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>810.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="7">
@@ -289,7 +289,7 @@
         <v>15</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>730.0</v>
+        <v>750.0</v>
       </c>
     </row>
     <row r="8">
@@ -300,7 +300,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>840.0</v>
+        <v>750.0</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
@@ -309,7 +309,7 @@
         <v>17</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>900.0</v>
+        <v>750.0</v>
       </c>
     </row>
     <row r="9">
@@ -325,7 +325,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>750.0</v>
+        <v>900.0</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>6</v>
@@ -334,7 +334,7 @@
         <v>17</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>900.0</v>
+        <v>750.0</v>
       </c>
     </row>
     <row r="11">
@@ -345,7 +345,7 @@
         <v>15</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>730.0</v>
+        <v>750.0</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>6</v>
@@ -354,7 +354,7 @@
         <v>16</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>840.0</v>
+        <v>750.0</v>
       </c>
     </row>
     <row r="12">
@@ -365,7 +365,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>810.0</v>
+        <v>0.0</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>6</v>
@@ -385,7 +385,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>750.0</v>
+        <v>720.0</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>6</v>
@@ -394,7 +394,7 @@
         <v>12</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>680.0</v>
+        <v>800.0</v>
       </c>
     </row>
     <row r="14">
@@ -405,7 +405,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>750.0</v>
+        <v>680.0</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>6</v>
@@ -414,7 +414,7 @@
         <v>10</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>800.0</v>
+        <v>810.0</v>
       </c>
     </row>
     <row r="15">
@@ -425,7 +425,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>0.0</v>
+        <v>840.0</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>6</v>
@@ -434,7 +434,7 @@
         <v>8</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>720.0</v>
+        <v>730.0</v>
       </c>
     </row>
     <row r="16">
@@ -450,7 +450,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>720.0</v>
+        <v>730.0</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>6</v>
@@ -459,7 +459,7 @@
         <v>7</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>750.0</v>
+        <v>900.0</v>
       </c>
     </row>
     <row r="18">
@@ -470,7 +470,7 @@
         <v>10</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>800.0</v>
+        <v>810.0</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>6</v>
@@ -479,7 +479,7 @@
         <v>5</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>0.0</v>
+        <v>840.0</v>
       </c>
     </row>
     <row r="19">
@@ -490,7 +490,7 @@
         <v>12</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>680.0</v>
+        <v>800.0</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>6</v>
@@ -499,7 +499,7 @@
         <v>9</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>750.0</v>
+        <v>680.0</v>
       </c>
     </row>
     <row r="20">
@@ -519,7 +519,7 @@
         <v>11</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>750.0</v>
+        <v>720.0</v>
       </c>
     </row>
     <row r="21">
@@ -530,7 +530,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>840.0</v>
+        <v>750.0</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>6</v>
@@ -539,7 +539,7 @@
         <v>13</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>810.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="22">
@@ -550,7 +550,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>900.0</v>
+        <v>750.0</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>6</v>
@@ -559,7 +559,7 @@
         <v>15</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>730.0</v>
+        <v>750.0</v>
       </c>
     </row>
     <row r="23">
@@ -575,7 +575,7 @@
         <v>7</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>750.0</v>
+        <v>900.0</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>6</v>
@@ -584,7 +584,7 @@
         <v>15</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>730.0</v>
+        <v>750.0</v>
       </c>
     </row>
     <row r="25">
@@ -595,7 +595,7 @@
         <v>13</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>810.0</v>
+        <v>0.0</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>6</v>
@@ -604,7 +604,7 @@
         <v>17</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>900.0</v>
+        <v>750.0</v>
       </c>
     </row>
     <row r="26">
@@ -615,7 +615,7 @@
         <v>11</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>750.0</v>
+        <v>720.0</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>6</v>
@@ -624,7 +624,7 @@
         <v>16</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>840.0</v>
+        <v>750.0</v>
       </c>
     </row>
     <row r="27">
@@ -635,7 +635,7 @@
         <v>9</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>750.0</v>
+        <v>680.0</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>6</v>
@@ -655,7 +655,7 @@
         <v>5</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>0.0</v>
+        <v>840.0</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>6</v>
@@ -664,7 +664,7 @@
         <v>12</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>680.0</v>
+        <v>800.0</v>
       </c>
     </row>
     <row r="29">
@@ -675,7 +675,7 @@
         <v>8</v>
       </c>
       <c r="C29" s="2" t="n">
-        <v>720.0</v>
+        <v>730.0</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>6</v>
@@ -684,7 +684,7 @@
         <v>10</v>
       </c>
       <c r="F29" s="2" t="n">
-        <v>800.0</v>
+        <v>810.0</v>
       </c>
     </row>
     <row r="30">
@@ -700,7 +700,7 @@
         <v>10</v>
       </c>
       <c r="C31" s="2" t="n">
-        <v>800.0</v>
+        <v>810.0</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>6</v>
@@ -709,7 +709,7 @@
         <v>7</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>750.0</v>
+        <v>900.0</v>
       </c>
     </row>
     <row r="32">
@@ -720,7 +720,7 @@
         <v>12</v>
       </c>
       <c r="C32" s="2" t="n">
-        <v>680.0</v>
+        <v>800.0</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>6</v>
@@ -729,7 +729,7 @@
         <v>8</v>
       </c>
       <c r="F32" s="2" t="n">
-        <v>720.0</v>
+        <v>730.0</v>
       </c>
     </row>
     <row r="33">
@@ -749,7 +749,7 @@
         <v>5</v>
       </c>
       <c r="F33" s="2" t="n">
-        <v>0.0</v>
+        <v>840.0</v>
       </c>
     </row>
     <row r="34">
@@ -760,7 +760,7 @@
         <v>16</v>
       </c>
       <c r="C34" s="2" t="n">
-        <v>840.0</v>
+        <v>750.0</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>6</v>
@@ -769,7 +769,7 @@
         <v>9</v>
       </c>
       <c r="F34" s="2" t="n">
-        <v>750.0</v>
+        <v>680.0</v>
       </c>
     </row>
     <row r="35">
@@ -780,7 +780,7 @@
         <v>17</v>
       </c>
       <c r="C35" s="2" t="n">
-        <v>900.0</v>
+        <v>750.0</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>6</v>
@@ -789,7 +789,7 @@
         <v>11</v>
       </c>
       <c r="F35" s="2" t="n">
-        <v>750.0</v>
+        <v>720.0</v>
       </c>
     </row>
     <row r="36">
@@ -800,7 +800,7 @@
         <v>15</v>
       </c>
       <c r="C36" s="2" t="n">
-        <v>730.0</v>
+        <v>750.0</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>6</v>
@@ -809,7 +809,7 @@
         <v>13</v>
       </c>
       <c r="F36" s="2" t="n">
-        <v>810.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="37">
@@ -825,7 +825,7 @@
         <v>7</v>
       </c>
       <c r="C38" s="2" t="n">
-        <v>750.0</v>
+        <v>900.0</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>6</v>
@@ -834,7 +834,7 @@
         <v>13</v>
       </c>
       <c r="F38" s="2" t="n">
-        <v>810.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="39">
@@ -845,7 +845,7 @@
         <v>11</v>
       </c>
       <c r="C39" s="2" t="n">
-        <v>750.0</v>
+        <v>720.0</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>6</v>
@@ -854,7 +854,7 @@
         <v>15</v>
       </c>
       <c r="F39" s="2" t="n">
-        <v>730.0</v>
+        <v>750.0</v>
       </c>
     </row>
     <row r="40">
@@ -865,7 +865,7 @@
         <v>9</v>
       </c>
       <c r="C40" s="2" t="n">
-        <v>750.0</v>
+        <v>680.0</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>6</v>
@@ -874,7 +874,7 @@
         <v>17</v>
       </c>
       <c r="F40" s="2" t="n">
-        <v>900.0</v>
+        <v>750.0</v>
       </c>
     </row>
     <row r="41">
@@ -885,7 +885,7 @@
         <v>5</v>
       </c>
       <c r="C41" s="2" t="n">
-        <v>0.0</v>
+        <v>840.0</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>6</v>
@@ -894,7 +894,7 @@
         <v>16</v>
       </c>
       <c r="F41" s="2" t="n">
-        <v>840.0</v>
+        <v>750.0</v>
       </c>
     </row>
     <row r="42">
@@ -905,7 +905,7 @@
         <v>8</v>
       </c>
       <c r="C42" s="2" t="n">
-        <v>720.0</v>
+        <v>730.0</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>6</v>
@@ -925,7 +925,7 @@
         <v>10</v>
       </c>
       <c r="C43" s="2" t="n">
-        <v>800.0</v>
+        <v>810.0</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>6</v>
@@ -934,7 +934,7 @@
         <v>12</v>
       </c>
       <c r="F43" s="2" t="n">
-        <v>680.0</v>
+        <v>800.0</v>
       </c>
     </row>
     <row r="44">
@@ -950,7 +950,7 @@
         <v>12</v>
       </c>
       <c r="C45" s="2" t="n">
-        <v>680.0</v>
+        <v>800.0</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>6</v>
@@ -959,7 +959,7 @@
         <v>7</v>
       </c>
       <c r="F45" s="2" t="n">
-        <v>750.0</v>
+        <v>900.0</v>
       </c>
     </row>
     <row r="46">
@@ -979,7 +979,7 @@
         <v>10</v>
       </c>
       <c r="F46" s="2" t="n">
-        <v>800.0</v>
+        <v>810.0</v>
       </c>
     </row>
     <row r="47">
@@ -990,7 +990,7 @@
         <v>16</v>
       </c>
       <c r="C47" s="2" t="n">
-        <v>840.0</v>
+        <v>750.0</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>6</v>
@@ -999,7 +999,7 @@
         <v>8</v>
       </c>
       <c r="F47" s="2" t="n">
-        <v>720.0</v>
+        <v>730.0</v>
       </c>
     </row>
     <row r="48">
@@ -1010,7 +1010,7 @@
         <v>17</v>
       </c>
       <c r="C48" s="2" t="n">
-        <v>900.0</v>
+        <v>750.0</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>6</v>
@@ -1019,7 +1019,7 @@
         <v>5</v>
       </c>
       <c r="F48" s="2" t="n">
-        <v>0.0</v>
+        <v>840.0</v>
       </c>
     </row>
     <row r="49">
@@ -1030,7 +1030,7 @@
         <v>15</v>
       </c>
       <c r="C49" s="2" t="n">
-        <v>730.0</v>
+        <v>750.0</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>6</v>
@@ -1039,7 +1039,7 @@
         <v>9</v>
       </c>
       <c r="F49" s="2" t="n">
-        <v>750.0</v>
+        <v>680.0</v>
       </c>
     </row>
     <row r="50">
@@ -1050,7 +1050,7 @@
         <v>13</v>
       </c>
       <c r="C50" s="2" t="n">
-        <v>810.0</v>
+        <v>0.0</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>6</v>
@@ -1059,7 +1059,7 @@
         <v>11</v>
       </c>
       <c r="F50" s="2" t="n">
-        <v>750.0</v>
+        <v>720.0</v>
       </c>
     </row>
     <row r="51">
@@ -1075,7 +1075,7 @@
         <v>7</v>
       </c>
       <c r="C52" s="2" t="n">
-        <v>750.0</v>
+        <v>900.0</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>6</v>
@@ -1084,7 +1084,7 @@
         <v>11</v>
       </c>
       <c r="F52" s="2" t="n">
-        <v>750.0</v>
+        <v>720.0</v>
       </c>
     </row>
     <row r="53">
@@ -1095,7 +1095,7 @@
         <v>9</v>
       </c>
       <c r="C53" s="2" t="n">
-        <v>750.0</v>
+        <v>680.0</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>6</v>
@@ -1104,7 +1104,7 @@
         <v>13</v>
       </c>
       <c r="F53" s="2" t="n">
-        <v>810.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="54">
@@ -1115,7 +1115,7 @@
         <v>5</v>
       </c>
       <c r="C54" s="2" t="n">
-        <v>0.0</v>
+        <v>840.0</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>6</v>
@@ -1124,7 +1124,7 @@
         <v>15</v>
       </c>
       <c r="F54" s="2" t="n">
-        <v>730.0</v>
+        <v>750.0</v>
       </c>
     </row>
     <row r="55">
@@ -1135,7 +1135,7 @@
         <v>8</v>
       </c>
       <c r="C55" s="2" t="n">
-        <v>720.0</v>
+        <v>730.0</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>6</v>
@@ -1144,7 +1144,7 @@
         <v>17</v>
       </c>
       <c r="F55" s="2" t="n">
-        <v>900.0</v>
+        <v>750.0</v>
       </c>
     </row>
     <row r="56">
@@ -1155,7 +1155,7 @@
         <v>10</v>
       </c>
       <c r="C56" s="2" t="n">
-        <v>800.0</v>
+        <v>810.0</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>6</v>
@@ -1164,7 +1164,7 @@
         <v>16</v>
       </c>
       <c r="F56" s="2" t="n">
-        <v>840.0</v>
+        <v>750.0</v>
       </c>
     </row>
     <row r="57">
@@ -1175,7 +1175,7 @@
         <v>12</v>
       </c>
       <c r="C57" s="2" t="n">
-        <v>680.0</v>
+        <v>800.0</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>6</v>
@@ -1209,7 +1209,7 @@
         <v>7</v>
       </c>
       <c r="F59" s="2" t="n">
-        <v>750.0</v>
+        <v>900.0</v>
       </c>
     </row>
     <row r="60">
@@ -1220,7 +1220,7 @@
         <v>16</v>
       </c>
       <c r="C60" s="2" t="n">
-        <v>840.0</v>
+        <v>750.0</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>6</v>
@@ -1229,7 +1229,7 @@
         <v>12</v>
       </c>
       <c r="F60" s="2" t="n">
-        <v>680.0</v>
+        <v>800.0</v>
       </c>
     </row>
     <row r="61">
@@ -1240,7 +1240,7 @@
         <v>17</v>
       </c>
       <c r="C61" s="2" t="n">
-        <v>900.0</v>
+        <v>750.0</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>6</v>
@@ -1249,7 +1249,7 @@
         <v>10</v>
       </c>
       <c r="F61" s="2" t="n">
-        <v>800.0</v>
+        <v>810.0</v>
       </c>
     </row>
     <row r="62">
@@ -1260,7 +1260,7 @@
         <v>15</v>
       </c>
       <c r="C62" s="2" t="n">
-        <v>730.0</v>
+        <v>750.0</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>6</v>
@@ -1269,7 +1269,7 @@
         <v>8</v>
       </c>
       <c r="F62" s="2" t="n">
-        <v>720.0</v>
+        <v>730.0</v>
       </c>
     </row>
     <row r="63">
@@ -1280,7 +1280,7 @@
         <v>13</v>
       </c>
       <c r="C63" s="2" t="n">
-        <v>810.0</v>
+        <v>0.0</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>6</v>
@@ -1289,7 +1289,7 @@
         <v>5</v>
       </c>
       <c r="F63" s="2" t="n">
-        <v>0.0</v>
+        <v>840.0</v>
       </c>
     </row>
     <row r="64">
@@ -1300,7 +1300,7 @@
         <v>11</v>
       </c>
       <c r="C64" s="2" t="n">
-        <v>750.0</v>
+        <v>720.0</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>6</v>
@@ -1309,7 +1309,7 @@
         <v>9</v>
       </c>
       <c r="F64" s="2" t="n">
-        <v>750.0</v>
+        <v>680.0</v>
       </c>
     </row>
     <row r="65">
@@ -1325,7 +1325,7 @@
         <v>7</v>
       </c>
       <c r="C66" s="2" t="n">
-        <v>750.0</v>
+        <v>900.0</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>6</v>
@@ -1334,7 +1334,7 @@
         <v>9</v>
       </c>
       <c r="F66" s="2" t="n">
-        <v>750.0</v>
+        <v>680.0</v>
       </c>
     </row>
     <row r="67">
@@ -1345,7 +1345,7 @@
         <v>5</v>
       </c>
       <c r="C67" s="2" t="n">
-        <v>0.0</v>
+        <v>840.0</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>6</v>
@@ -1354,7 +1354,7 @@
         <v>11</v>
       </c>
       <c r="F67" s="2" t="n">
-        <v>750.0</v>
+        <v>720.0</v>
       </c>
     </row>
     <row r="68">
@@ -1365,7 +1365,7 @@
         <v>8</v>
       </c>
       <c r="C68" s="2" t="n">
-        <v>720.0</v>
+        <v>730.0</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>6</v>
@@ -1374,7 +1374,7 @@
         <v>13</v>
       </c>
       <c r="F68" s="2" t="n">
-        <v>810.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="69">
@@ -1385,7 +1385,7 @@
         <v>10</v>
       </c>
       <c r="C69" s="2" t="n">
-        <v>800.0</v>
+        <v>810.0</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>6</v>
@@ -1394,7 +1394,7 @@
         <v>15</v>
       </c>
       <c r="F69" s="2" t="n">
-        <v>730.0</v>
+        <v>750.0</v>
       </c>
     </row>
     <row r="70">
@@ -1405,7 +1405,7 @@
         <v>12</v>
       </c>
       <c r="C70" s="2" t="n">
-        <v>680.0</v>
+        <v>800.0</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>6</v>
@@ -1414,7 +1414,7 @@
         <v>17</v>
       </c>
       <c r="F70" s="2" t="n">
-        <v>900.0</v>
+        <v>750.0</v>
       </c>
     </row>
     <row r="71">
@@ -1434,7 +1434,7 @@
         <v>16</v>
       </c>
       <c r="F71" s="2" t="n">
-        <v>840.0</v>
+        <v>750.0</v>
       </c>
     </row>
     <row r="72">
@@ -1450,7 +1450,7 @@
         <v>16</v>
       </c>
       <c r="C73" s="2" t="n">
-        <v>840.0</v>
+        <v>750.0</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>6</v>
@@ -1459,7 +1459,7 @@
         <v>7</v>
       </c>
       <c r="F73" s="2" t="n">
-        <v>750.0</v>
+        <v>900.0</v>
       </c>
     </row>
     <row r="74">
@@ -1470,7 +1470,7 @@
         <v>17</v>
       </c>
       <c r="C74" s="2" t="n">
-        <v>900.0</v>
+        <v>750.0</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>6</v>
@@ -1490,7 +1490,7 @@
         <v>15</v>
       </c>
       <c r="C75" s="2" t="n">
-        <v>730.0</v>
+        <v>750.0</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>6</v>
@@ -1499,7 +1499,7 @@
         <v>12</v>
       </c>
       <c r="F75" s="2" t="n">
-        <v>680.0</v>
+        <v>800.0</v>
       </c>
     </row>
     <row r="76">
@@ -1510,7 +1510,7 @@
         <v>13</v>
       </c>
       <c r="C76" s="2" t="n">
-        <v>810.0</v>
+        <v>0.0</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>6</v>
@@ -1519,7 +1519,7 @@
         <v>10</v>
       </c>
       <c r="F76" s="2" t="n">
-        <v>800.0</v>
+        <v>810.0</v>
       </c>
     </row>
     <row r="77">
@@ -1530,7 +1530,7 @@
         <v>11</v>
       </c>
       <c r="C77" s="2" t="n">
-        <v>750.0</v>
+        <v>720.0</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>6</v>
@@ -1539,7 +1539,7 @@
         <v>8</v>
       </c>
       <c r="F77" s="2" t="n">
-        <v>720.0</v>
+        <v>730.0</v>
       </c>
     </row>
     <row r="78">
@@ -1550,7 +1550,7 @@
         <v>9</v>
       </c>
       <c r="C78" s="2" t="n">
-        <v>750.0</v>
+        <v>680.0</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>6</v>
@@ -1559,7 +1559,7 @@
         <v>5</v>
       </c>
       <c r="F78" s="2" t="n">
-        <v>0.0</v>
+        <v>840.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>